<commit_message>
Non exercise sessions API and persistence done
</commit_message>
<xml_diff>
--- a/doc/external-libraries.xlsx
+++ b/doc/external-libraries.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandeep/projects/sconsole/SConsoleNxt/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87E9E61-41EC-6C45-9BDE-2F190A7FA2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA316BBE-4595-4243-BB46-9513E105F17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4780" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{A6983AAA-76E0-C546-86DD-E7128BD6E8D3}"/>
+    <workbookView xWindow="4780" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{A6983AAA-76E0-C546-86DD-E7128BD6E8D3}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 01 18" sheetId="1" r:id="rId1"/>
+    <sheet name="2025 02 26" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="110">
   <si>
     <t>Server Libs</t>
   </si>
@@ -360,6 +361,12 @@
   </si>
   <si>
     <t>Introduced to process YAML</t>
+  </si>
+  <si>
+    <t>mapstruct-1.6.3.jar</t>
+  </si>
+  <si>
+    <t>MapStruct annotation processor introduced</t>
   </si>
 </sst>
 </file>
@@ -416,7 +423,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -444,6 +451,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -779,7 +796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDC4ED2-C3C0-9D4D-BFE6-B8567331BB0C}">
   <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -808,7 +825,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="b">
-        <f>B2=A2</f>
+        <f t="shared" ref="C2:C29" si="0">B2=A2</f>
         <v>1</v>
       </c>
     </row>
@@ -820,7 +837,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="b">
-        <f>B3=A3</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -832,7 +849,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="b">
-        <f>B4=A4</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -844,7 +861,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="b">
-        <f>B5=A5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -856,7 +873,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="b">
-        <f>B6=A6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -868,7 +885,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="b">
-        <f>B7=A7</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -880,7 +897,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="b">
-        <f>B8=A8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -892,7 +909,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="b">
-        <f>B9=A9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -904,7 +921,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="b">
-        <f>B10=A10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -916,7 +933,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="b">
-        <f>B11=A11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -928,7 +945,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="b">
-        <f>B12=A12</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -940,7 +957,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="b">
-        <f>B13=A13</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -952,7 +969,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="b">
-        <f>B14=A14</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -964,7 +981,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="b">
-        <f>B15=A15</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -976,7 +993,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="b">
-        <f>B16=A16</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -988,7 +1005,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="b">
-        <f>B17=A17</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1000,7 +1017,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="b">
-        <f>B18=A18</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1012,7 +1029,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="b">
-        <f>B19=A19</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1024,7 +1041,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="b">
-        <f>B20=A20</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1036,7 +1053,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="b">
-        <f>B21=A21</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1048,7 +1065,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="b">
-        <f>B22=A22</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1060,7 +1077,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="b">
-        <f>B23=A23</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1072,7 +1089,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="b">
-        <f>B24=A24</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1084,7 +1101,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="b">
-        <f>B25=A25</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1096,7 +1113,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="b">
-        <f>B26=A26</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1108,7 +1125,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="b">
-        <f>B27=A27</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1120,7 +1137,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="b">
-        <f>B28=A28</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1132,7 +1149,7 @@
         <v>28</v>
       </c>
       <c r="C29" t="b">
-        <f>B29=A29</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1142,7 +1159,7 @@
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="b">
-        <f t="shared" ref="C30:C93" si="0">B30=A30</f>
+        <f t="shared" ref="C30:C93" si="1">B30=A30</f>
         <v>0</v>
       </c>
       <c r="E30" t="s">
@@ -1157,7 +1174,7 @@
         <v>29</v>
       </c>
       <c r="C31" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1169,7 +1186,7 @@
         <v>30</v>
       </c>
       <c r="C32" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1181,7 +1198,7 @@
         <v>31</v>
       </c>
       <c r="C33" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1193,7 +1210,7 @@
         <v>32</v>
       </c>
       <c r="C34" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1205,7 +1222,7 @@
         <v>33</v>
       </c>
       <c r="C35" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1217,7 +1234,7 @@
         <v>34</v>
       </c>
       <c r="C36" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1229,7 +1246,7 @@
         <v>35</v>
       </c>
       <c r="C37" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1241,7 +1258,7 @@
         <v>36</v>
       </c>
       <c r="C38" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1253,7 +1270,7 @@
         <v>37</v>
       </c>
       <c r="C39" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1265,7 +1282,7 @@
         <v>38</v>
       </c>
       <c r="C40" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1277,7 +1294,7 @@
         <v>39</v>
       </c>
       <c r="C41" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1289,7 +1306,7 @@
         <v>40</v>
       </c>
       <c r="C42" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1301,7 +1318,7 @@
         <v>41</v>
       </c>
       <c r="C43" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1313,7 +1330,7 @@
         <v>42</v>
       </c>
       <c r="C44" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1325,7 +1342,7 @@
         <v>43</v>
       </c>
       <c r="C45" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1337,7 +1354,7 @@
         <v>44</v>
       </c>
       <c r="C46" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1349,7 +1366,7 @@
         <v>45</v>
       </c>
       <c r="C47" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1361,7 +1378,7 @@
         <v>46</v>
       </c>
       <c r="C48" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1373,7 +1390,7 @@
         <v>47</v>
       </c>
       <c r="C49" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1385,7 +1402,7 @@
         <v>48</v>
       </c>
       <c r="C50" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1397,7 +1414,7 @@
         <v>49</v>
       </c>
       <c r="C51" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1409,7 +1426,7 @@
         <v>50</v>
       </c>
       <c r="C52" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1421,7 +1438,7 @@
         <v>51</v>
       </c>
       <c r="C53" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1433,7 +1450,7 @@
         <v>52</v>
       </c>
       <c r="C54" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1445,7 +1462,7 @@
         <v>53</v>
       </c>
       <c r="C55" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1457,7 +1474,7 @@
         <v>54</v>
       </c>
       <c r="C56" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1469,7 +1486,7 @@
         <v>55</v>
       </c>
       <c r="C57" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1481,7 +1498,7 @@
         <v>56</v>
       </c>
       <c r="C58" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1493,7 +1510,7 @@
         <v>57</v>
       </c>
       <c r="C59" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1505,7 +1522,7 @@
         <v>58</v>
       </c>
       <c r="C60" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1517,7 +1534,7 @@
         <v>59</v>
       </c>
       <c r="C61" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1529,7 +1546,7 @@
         <v>60</v>
       </c>
       <c r="C62" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1541,7 +1558,7 @@
         <v>61</v>
       </c>
       <c r="C63" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1553,7 +1570,7 @@
         <v>62</v>
       </c>
       <c r="C64" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1565,7 +1582,7 @@
         <v>63</v>
       </c>
       <c r="C65" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1577,7 +1594,7 @@
         <v>64</v>
       </c>
       <c r="C66" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1589,7 +1606,7 @@
         <v>65</v>
       </c>
       <c r="C67" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1601,7 +1618,7 @@
         <v>66</v>
       </c>
       <c r="C68" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1613,7 +1630,7 @@
         <v>67</v>
       </c>
       <c r="C69" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1625,7 +1642,7 @@
         <v>68</v>
       </c>
       <c r="C70" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1637,7 +1654,7 @@
         <v>69</v>
       </c>
       <c r="C71" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1649,7 +1666,7 @@
         <v>70</v>
       </c>
       <c r="C72" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1661,7 +1678,7 @@
         <v>71</v>
       </c>
       <c r="C73" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1673,7 +1690,7 @@
         <v>72</v>
       </c>
       <c r="C74" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1685,7 +1702,7 @@
         <v>73</v>
       </c>
       <c r="C75" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1697,7 +1714,7 @@
         <v>74</v>
       </c>
       <c r="C76" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1709,7 +1726,7 @@
         <v>75</v>
       </c>
       <c r="C77" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1721,7 +1738,7 @@
         <v>76</v>
       </c>
       <c r="C78" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1733,7 +1750,7 @@
         <v>77</v>
       </c>
       <c r="C79" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1745,7 +1762,7 @@
         <v>78</v>
       </c>
       <c r="C80" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1757,7 +1774,7 @@
         <v>79</v>
       </c>
       <c r="C81" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1769,7 +1786,7 @@
         <v>80</v>
       </c>
       <c r="C82" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1781,7 +1798,7 @@
         <v>81</v>
       </c>
       <c r="C83" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1793,7 +1810,7 @@
         <v>82</v>
       </c>
       <c r="C84" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1805,7 +1822,7 @@
         <v>83</v>
       </c>
       <c r="C85" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1817,7 +1834,7 @@
         <v>84</v>
       </c>
       <c r="C86" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1829,7 +1846,7 @@
         <v>85</v>
       </c>
       <c r="C87" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1841,7 +1858,7 @@
         <v>86</v>
       </c>
       <c r="C88" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1853,7 +1870,7 @@
         <v>87</v>
       </c>
       <c r="C89" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1865,7 +1882,7 @@
         <v>88</v>
       </c>
       <c r="C90" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1877,7 +1894,7 @@
         <v>89</v>
       </c>
       <c r="C91" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1889,7 +1906,7 @@
         <v>90</v>
       </c>
       <c r="C92" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1901,7 +1918,7 @@
         <v>91</v>
       </c>
       <c r="C93" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1913,7 +1930,7 @@
         <v>92</v>
       </c>
       <c r="C94" t="b">
-        <f t="shared" ref="C94:C105" si="1">B94=A94</f>
+        <f t="shared" ref="C94:C105" si="2">B94=A94</f>
         <v>1</v>
       </c>
     </row>
@@ -1925,7 +1942,7 @@
         <v>93</v>
       </c>
       <c r="C95" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1937,7 +1954,7 @@
         <v>94</v>
       </c>
       <c r="C96" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1949,7 +1966,7 @@
         <v>95</v>
       </c>
       <c r="C97" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1961,7 +1978,7 @@
         <v>96</v>
       </c>
       <c r="C98" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1973,7 +1990,7 @@
         <v>97</v>
       </c>
       <c r="C99" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1985,7 +2002,7 @@
         <v>98</v>
       </c>
       <c r="C100" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1997,7 +2014,7 @@
         <v>99</v>
       </c>
       <c r="C101" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2009,7 +2026,7 @@
         <v>100</v>
       </c>
       <c r="C102" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2021,7 +2038,7 @@
         <v>101</v>
       </c>
       <c r="C103" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2033,7 +2050,7 @@
         <v>102</v>
       </c>
       <c r="C104" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2045,12 +2062,1311 @@
         <v>103</v>
       </c>
       <c r="C105" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C105">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE6B34AD-51F6-7648-B82E-80DEA365162B}">
+  <dimension ref="A1:D106"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="55.83203125" customWidth="1"/>
+    <col min="2" max="2" width="45.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="b">
+        <f>B2=A2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="b">
+        <f t="shared" ref="C2:C65" si="0">B3=A3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C54" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D58" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>56</v>
+      </c>
+      <c r="B59" t="s">
+        <v>56</v>
+      </c>
+      <c r="C59" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60" t="s">
+        <v>57</v>
+      </c>
+      <c r="C60" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>58</v>
+      </c>
+      <c r="B61" t="s">
+        <v>58</v>
+      </c>
+      <c r="C61" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>59</v>
+      </c>
+      <c r="B62" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" t="s">
+        <v>60</v>
+      </c>
+      <c r="C63" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>61</v>
+      </c>
+      <c r="B64" t="s">
+        <v>61</v>
+      </c>
+      <c r="C64" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>62</v>
+      </c>
+      <c r="B65" t="s">
+        <v>62</v>
+      </c>
+      <c r="C65" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66" t="s">
+        <v>63</v>
+      </c>
+      <c r="C66" t="b">
+        <f t="shared" ref="C66:C106" si="1">B66=A66</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>64</v>
+      </c>
+      <c r="B67" t="s">
+        <v>64</v>
+      </c>
+      <c r="C67" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>65</v>
+      </c>
+      <c r="B68" t="s">
+        <v>65</v>
+      </c>
+      <c r="C68" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>66</v>
+      </c>
+      <c r="B69" t="s">
+        <v>66</v>
+      </c>
+      <c r="C69" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>67</v>
+      </c>
+      <c r="B70" t="s">
+        <v>67</v>
+      </c>
+      <c r="C70" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>68</v>
+      </c>
+      <c r="B71" t="s">
+        <v>68</v>
+      </c>
+      <c r="C71" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>69</v>
+      </c>
+      <c r="B72" t="s">
+        <v>69</v>
+      </c>
+      <c r="C72" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>70</v>
+      </c>
+      <c r="B73" t="s">
+        <v>70</v>
+      </c>
+      <c r="C73" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>71</v>
+      </c>
+      <c r="B74" t="s">
+        <v>71</v>
+      </c>
+      <c r="C74" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>72</v>
+      </c>
+      <c r="B75" t="s">
+        <v>72</v>
+      </c>
+      <c r="C75" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>73</v>
+      </c>
+      <c r="B76" t="s">
+        <v>73</v>
+      </c>
+      <c r="C76" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>74</v>
+      </c>
+      <c r="B77" t="s">
+        <v>74</v>
+      </c>
+      <c r="C77" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>75</v>
+      </c>
+      <c r="B78" t="s">
+        <v>75</v>
+      </c>
+      <c r="C78" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>76</v>
+      </c>
+      <c r="B79" t="s">
+        <v>76</v>
+      </c>
+      <c r="C79" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>77</v>
+      </c>
+      <c r="B80" t="s">
+        <v>77</v>
+      </c>
+      <c r="C80" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>78</v>
+      </c>
+      <c r="B81" t="s">
+        <v>78</v>
+      </c>
+      <c r="C81" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>79</v>
+      </c>
+      <c r="B82" t="s">
+        <v>79</v>
+      </c>
+      <c r="C82" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>80</v>
+      </c>
+      <c r="B83" t="s">
+        <v>80</v>
+      </c>
+      <c r="C83" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>81</v>
+      </c>
+      <c r="B84" t="s">
+        <v>81</v>
+      </c>
+      <c r="C84" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>82</v>
+      </c>
+      <c r="B85" t="s">
+        <v>82</v>
+      </c>
+      <c r="C85" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>83</v>
+      </c>
+      <c r="B86" t="s">
+        <v>83</v>
+      </c>
+      <c r="C86" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>84</v>
+      </c>
+      <c r="B87" t="s">
+        <v>84</v>
+      </c>
+      <c r="C87" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>85</v>
+      </c>
+      <c r="B88" t="s">
+        <v>85</v>
+      </c>
+      <c r="C88" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>86</v>
+      </c>
+      <c r="B89" t="s">
+        <v>86</v>
+      </c>
+      <c r="C89" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>87</v>
+      </c>
+      <c r="B90" t="s">
+        <v>87</v>
+      </c>
+      <c r="C90" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>88</v>
+      </c>
+      <c r="B91" t="s">
+        <v>88</v>
+      </c>
+      <c r="C91" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>89</v>
+      </c>
+      <c r="B92" t="s">
+        <v>89</v>
+      </c>
+      <c r="C92" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>90</v>
+      </c>
+      <c r="B93" t="s">
+        <v>90</v>
+      </c>
+      <c r="C93" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>91</v>
+      </c>
+      <c r="B94" t="s">
+        <v>91</v>
+      </c>
+      <c r="C94" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>92</v>
+      </c>
+      <c r="B95" t="s">
+        <v>92</v>
+      </c>
+      <c r="C95" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>93</v>
+      </c>
+      <c r="B96" t="s">
+        <v>93</v>
+      </c>
+      <c r="C96" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>94</v>
+      </c>
+      <c r="B97" t="s">
+        <v>94</v>
+      </c>
+      <c r="C97" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>95</v>
+      </c>
+      <c r="B98" t="s">
+        <v>95</v>
+      </c>
+      <c r="C98" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>96</v>
+      </c>
+      <c r="B99" t="s">
+        <v>96</v>
+      </c>
+      <c r="C99" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>97</v>
+      </c>
+      <c r="B100" t="s">
+        <v>97</v>
+      </c>
+      <c r="C100" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>98</v>
+      </c>
+      <c r="B101" t="s">
+        <v>98</v>
+      </c>
+      <c r="C101" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>99</v>
+      </c>
+      <c r="B102" t="s">
+        <v>99</v>
+      </c>
+      <c r="C102" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>100</v>
+      </c>
+      <c r="B103" t="s">
+        <v>100</v>
+      </c>
+      <c r="C103" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>101</v>
+      </c>
+      <c r="B104" t="s">
+        <v>101</v>
+      </c>
+      <c r="C104" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>102</v>
+      </c>
+      <c r="B105" t="s">
+        <v>102</v>
+      </c>
+      <c r="C105" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>103</v>
+      </c>
+      <c r="B106" t="s">
+        <v>103</v>
+      </c>
+      <c r="C106" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:C106">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
Remote screens coming up nicely
</commit_message>
<xml_diff>
--- a/doc/external-libraries.xlsx
+++ b/doc/external-libraries.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandeep/projects/sconsole/SConsoleNxt/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB55F3C-2D44-4646-A512-65045F751F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E3BE48-D6C3-DA43-AD9B-8A60A0AB35EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4780" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{A6983AAA-76E0-C546-86DD-E7128BD6E8D3}"/>
+    <workbookView xWindow="4780" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{A6983AAA-76E0-C546-86DD-E7128BD6E8D3}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 01 18" sheetId="1" r:id="rId1"/>
     <sheet name="2025 02 26" sheetId="2" r:id="rId2"/>
     <sheet name="2025 03 12" sheetId="3" r:id="rId3"/>
+    <sheet name="2025 03 13" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2025 03 12'!$A$1:$D$109</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2025 03 13'!$A$1:$D$99</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="122">
   <si>
     <t>Server Libs</t>
   </si>
@@ -386,6 +388,27 @@
   </si>
   <si>
     <t>Action</t>
+  </si>
+  <si>
+    <t>checker-qual-3.43.0.jar</t>
+  </si>
+  <si>
+    <t>error_prone_annotations-2.36.0.jar</t>
+  </si>
+  <si>
+    <t>failureaccess-1.0.2.jar</t>
+  </si>
+  <si>
+    <t>guava-33.4.0-jre.jar</t>
+  </si>
+  <si>
+    <t>j2objc-annotations-3.0.0.jar</t>
+  </si>
+  <si>
+    <t>jsr305-3.0.2.jar</t>
+  </si>
+  <si>
+    <t>listenablefuture-9999.0-empty-to-avoid-conflict-with-guava.jar</t>
   </si>
 </sst>
 </file>
@@ -452,18 +475,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2128,10 +2172,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C105">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3427,10 +3471,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C106">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3442,7 +3486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11956367-CD9C-EC4B-9F32-52680E70CD65}">
   <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -5158,6 +5202,1707 @@
   </sheetData>
   <autoFilter ref="A1:D109" xr:uid="{11956367-CD9C-EC4B-9F32-52680E70CD65}"/>
   <conditionalFormatting sqref="C2:C109">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30D0B58-1E58-054D-9ADA-A0DDCF33B3B5}">
+  <dimension ref="A1:D106"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.5" customWidth="1"/>
+    <col min="2" max="2" width="55.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="b">
+        <f>A2=B2</f>
+        <v>1</v>
+      </c>
+      <c r="D2" t="str">
+        <f>IF(A2=B2,"",IF(ISBLANK(A2),"DELETE","PUT"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="b">
+        <f t="shared" ref="C3:C66" si="0">A3=B3</f>
+        <v>1</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D66" si="1">IF(A3=B3,"",IF(ISBLANK(A3),"DELETE","PUT"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>PUT</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>PUT</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>PUT</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>PUT</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>PUT</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" t="s">
+        <v>42</v>
+      </c>
+      <c r="C46" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C47" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C50" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>120</v>
+      </c>
+      <c r="C52" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="1"/>
+        <v>PUT</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54" t="s">
+        <v>49</v>
+      </c>
+      <c r="C54" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="1"/>
+        <v>PUT</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>50</v>
+      </c>
+      <c r="B56" t="s">
+        <v>50</v>
+      </c>
+      <c r="C56" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>51</v>
+      </c>
+      <c r="B57" t="s">
+        <v>51</v>
+      </c>
+      <c r="C57" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>52</v>
+      </c>
+      <c r="B58" t="s">
+        <v>52</v>
+      </c>
+      <c r="C58" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59" t="s">
+        <v>53</v>
+      </c>
+      <c r="C59" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>54</v>
+      </c>
+      <c r="B60" t="s">
+        <v>54</v>
+      </c>
+      <c r="C60" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>55</v>
+      </c>
+      <c r="B61" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>56</v>
+      </c>
+      <c r="B62" t="s">
+        <v>56</v>
+      </c>
+      <c r="C62" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>57</v>
+      </c>
+      <c r="B63" t="s">
+        <v>57</v>
+      </c>
+      <c r="C63" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>58</v>
+      </c>
+      <c r="B64" t="s">
+        <v>58</v>
+      </c>
+      <c r="C64" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65" t="s">
+        <v>59</v>
+      </c>
+      <c r="C65" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>60</v>
+      </c>
+      <c r="B66" t="s">
+        <v>60</v>
+      </c>
+      <c r="C66" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>61</v>
+      </c>
+      <c r="B67" t="s">
+        <v>61</v>
+      </c>
+      <c r="C67" t="b">
+        <f t="shared" ref="C67:C106" si="2">A67=B67</f>
+        <v>1</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" ref="D67:D106" si="3">IF(A67=B67,"",IF(ISBLANK(A67),"DELETE","PUT"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>62</v>
+      </c>
+      <c r="B68" t="s">
+        <v>62</v>
+      </c>
+      <c r="C68" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>63</v>
+      </c>
+      <c r="B69" t="s">
+        <v>63</v>
+      </c>
+      <c r="C69" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>68</v>
+      </c>
+      <c r="C70" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>69</v>
+      </c>
+      <c r="C71" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>70</v>
+      </c>
+      <c r="C72" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>72</v>
+      </c>
+      <c r="C73" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>73</v>
+      </c>
+      <c r="C74" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>74</v>
+      </c>
+      <c r="C75" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>75</v>
+      </c>
+      <c r="C76" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>76</v>
+      </c>
+      <c r="C77" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>77</v>
+      </c>
+      <c r="C78" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>78</v>
+      </c>
+      <c r="C79" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>79</v>
+      </c>
+      <c r="C80" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>80</v>
+      </c>
+      <c r="C81" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>81</v>
+      </c>
+      <c r="C82" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>82</v>
+      </c>
+      <c r="C83" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>83</v>
+      </c>
+      <c r="C84" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>84</v>
+      </c>
+      <c r="C85" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>85</v>
+      </c>
+      <c r="C86" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>110</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C87" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>86</v>
+      </c>
+      <c r="C88" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>87</v>
+      </c>
+      <c r="C89" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>88</v>
+      </c>
+      <c r="C90" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>89</v>
+      </c>
+      <c r="C91" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>90</v>
+      </c>
+      <c r="C92" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>91</v>
+      </c>
+      <c r="C93" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>92</v>
+      </c>
+      <c r="C94" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>111</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C95" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>93</v>
+      </c>
+      <c r="B96" t="s">
+        <v>93</v>
+      </c>
+      <c r="C96" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>94</v>
+      </c>
+      <c r="B97" t="s">
+        <v>94</v>
+      </c>
+      <c r="C97" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>95</v>
+      </c>
+      <c r="B98" t="s">
+        <v>95</v>
+      </c>
+      <c r="C98" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>96</v>
+      </c>
+      <c r="B99" t="s">
+        <v>96</v>
+      </c>
+      <c r="C99" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>112</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C100" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>97</v>
+      </c>
+      <c r="B101" t="s">
+        <v>97</v>
+      </c>
+      <c r="C101" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>98</v>
+      </c>
+      <c r="B102" t="s">
+        <v>98</v>
+      </c>
+      <c r="C102" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D102" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>99</v>
+      </c>
+      <c r="B103" t="s">
+        <v>99</v>
+      </c>
+      <c r="C103" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D103" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>100</v>
+      </c>
+      <c r="B104" t="s">
+        <v>100</v>
+      </c>
+      <c r="C104" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>101</v>
+      </c>
+      <c r="B105" t="s">
+        <v>101</v>
+      </c>
+      <c r="C105" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D105" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>102</v>
+      </c>
+      <c r="B106" t="s">
+        <v>102</v>
+      </c>
+      <c r="C106" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D99" xr:uid="{11956367-CD9C-EC4B-9F32-52680E70CD65}"/>
+  <conditionalFormatting sqref="C2:C106">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
ChemSpider API integration deployed in production.
</commit_message>
<xml_diff>
--- a/doc/external-libraries.xlsx
+++ b/doc/external-libraries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandeep/projects/sconsole/SConsoleNxt/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7271A704-A0C8-FB4E-9013-6B208D07F6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8AF03F-2C31-AA43-B07C-36D172AA6245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="38400" windowHeight="24000" activeTab="5" xr2:uid="{A6983AAA-76E0-C546-86DD-E7128BD6E8D3}"/>
+    <workbookView xWindow="4780" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{A6983AAA-76E0-C546-86DD-E7128BD6E8D3}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 01 18" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,16 @@
     <sheet name="2025 03 12" sheetId="3" r:id="rId3"/>
     <sheet name="2025 03 13" sheetId="4" r:id="rId4"/>
     <sheet name="2025 06 02" sheetId="6" r:id="rId5"/>
-    <sheet name="next" sheetId="8" r:id="rId6"/>
+    <sheet name="2025 09 09" sheetId="8" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2025 03 12'!$A$1:$D$109</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2025 03 13'!$A$1:$D$99</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'2025 06 02'!$A$1:$D$108</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">next!$A$1:$D$108</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'2025 09 09'!$A$1:$D$108</definedName>
     <definedName name="libraries" localSheetId="4">'2025 06 02'!$A$2:$A$108</definedName>
-    <definedName name="libraries" localSheetId="5">next!$A$2:$A$108</definedName>
+    <definedName name="libraries" localSheetId="5">'2025 09 09'!$B$2:$B$111</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,14 +52,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{79C2282E-CEF9-1A49-8925-F5FB8A4486F4}" name="libraries" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/sandeep/projects/sconsole/SConsoleNxt/target/sconsole-1.0/lib/libraries.txt">
+    <textPr sourceFile="/Users/sandeep/projects/sconsole/SConsoleNxt/target/sconsole-1.0/lib/libraries.txt">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{A7D4C283-5746-7143-8CD1-E5005B60F952}" name="libraries1" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/sandeep/projects/sconsole/SConsoleNxt/target/sconsole-1.0/lib/libraries.txt">
+    <textPr sourceFile="/Users/sandeep/projects/sconsole/SConsoleNxt/target/sconsole-1.0/lib/libraries.txt">
       <textFields>
         <textField/>
       </textFields>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="190">
   <si>
     <t>Server Libs</t>
   </si>
@@ -623,6 +624,21 @@
   </si>
   <si>
     <t>txw2-4.0.5.jar</t>
+  </si>
+  <si>
+    <t>indigo-1.34.0.jar</t>
+  </si>
+  <si>
+    <t>indigo-renderer-1.34.0.jar</t>
+  </si>
+  <si>
+    <t>jna-5.12.1.jar</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>Server</t>
   </si>
 </sst>
 </file>
@@ -700,7 +716,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2433,10 +2469,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C105">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3732,10 +3768,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C106">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5463,10 +5499,10 @@
   </sheetData>
   <autoFilter ref="A1:D109" xr:uid="{11956367-CD9C-EC4B-9F32-52680E70CD65}"/>
   <conditionalFormatting sqref="C2:C109">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7164,10 +7200,10 @@
   </sheetData>
   <autoFilter ref="A1:D99" xr:uid="{11956367-CD9C-EC4B-9F32-52680E70CD65}"/>
   <conditionalFormatting sqref="C2:C106">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7179,7 +7215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D493EE-FA75-8743-8B46-178C51B1FF47}">
   <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A106" workbookViewId="0">
       <selection activeCell="H116" sqref="H116"/>
     </sheetView>
   </sheetViews>
@@ -9230,6 +9266,1799 @@
   </sheetData>
   <autoFilter ref="A1:D108" xr:uid="{11956367-CD9C-EC4B-9F32-52680E70CD65}"/>
   <conditionalFormatting sqref="C2:C108">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE4332B-3F41-D74D-BC46-926B80854FC8}">
+  <dimension ref="A1:D111"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="53.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="b">
+        <f>A2=B2</f>
+        <v>1</v>
+      </c>
+      <c r="D2" t="str">
+        <f>IF(A2=B2,"",IF(ISBLANK(B2),"PUT","DELETE"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="b">
+        <f t="shared" ref="C3:C66" si="0">A3=B3</f>
+        <v>1</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D66" si="1">IF(A3=B3,"",IF(ISBLANK(B3),"PUT","DELETE"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>185</v>
+      </c>
+      <c r="C28" t="b">
+        <f t="shared" ref="C28:C91" si="2">A28=B28</f>
+        <v>0</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>PUT</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>186</v>
+      </c>
+      <c r="C29" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>PUT</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" t="s">
+        <v>119</v>
+      </c>
+      <c r="C31" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" t="s">
+        <v>130</v>
+      </c>
+      <c r="C32" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" t="s">
+        <v>131</v>
+      </c>
+      <c r="C33" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>133</v>
+      </c>
+      <c r="B35" t="s">
+        <v>133</v>
+      </c>
+      <c r="C35" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36" t="s">
+        <v>134</v>
+      </c>
+      <c r="C36" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>136</v>
+      </c>
+      <c r="B38" t="s">
+        <v>136</v>
+      </c>
+      <c r="C38" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>137</v>
+      </c>
+      <c r="B39" t="s">
+        <v>137</v>
+      </c>
+      <c r="C39" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>138</v>
+      </c>
+      <c r="B44" t="s">
+        <v>138</v>
+      </c>
+      <c r="C44" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>139</v>
+      </c>
+      <c r="B45" t="s">
+        <v>139</v>
+      </c>
+      <c r="C45" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>140</v>
+      </c>
+      <c r="B48" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>141</v>
+      </c>
+      <c r="B49" t="s">
+        <v>141</v>
+      </c>
+      <c r="C49" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>142</v>
+      </c>
+      <c r="B52" t="s">
+        <v>142</v>
+      </c>
+      <c r="C52" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>187</v>
+      </c>
+      <c r="C54" t="b">
+        <f t="shared" ref="C54:C111" si="3">A54=B54</f>
+        <v>0</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="1"/>
+        <v>PUT</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>47</v>
+      </c>
+      <c r="B55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" t="s">
+        <v>120</v>
+      </c>
+      <c r="C56" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>143</v>
+      </c>
+      <c r="B57" t="s">
+        <v>143</v>
+      </c>
+      <c r="C57" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>49</v>
+      </c>
+      <c r="B58" t="s">
+        <v>49</v>
+      </c>
+      <c r="C58" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>121</v>
+      </c>
+      <c r="B59" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>50</v>
+      </c>
+      <c r="B60" t="s">
+        <v>50</v>
+      </c>
+      <c r="C60" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>144</v>
+      </c>
+      <c r="B61" t="s">
+        <v>144</v>
+      </c>
+      <c r="C61" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>145</v>
+      </c>
+      <c r="B62" t="s">
+        <v>145</v>
+      </c>
+      <c r="C62" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>146</v>
+      </c>
+      <c r="B63" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>147</v>
+      </c>
+      <c r="B64" t="s">
+        <v>147</v>
+      </c>
+      <c r="C64" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>55</v>
+      </c>
+      <c r="B65" t="s">
+        <v>55</v>
+      </c>
+      <c r="C65" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>148</v>
+      </c>
+      <c r="B66" t="s">
+        <v>148</v>
+      </c>
+      <c r="C66" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>149</v>
+      </c>
+      <c r="B67" t="s">
+        <v>149</v>
+      </c>
+      <c r="C67" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" ref="D67:D111" si="4">IF(A67=B67,"",IF(ISBLANK(B67),"PUT","DELETE"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>58</v>
+      </c>
+      <c r="B68" t="s">
+        <v>58</v>
+      </c>
+      <c r="C68" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>59</v>
+      </c>
+      <c r="B69" t="s">
+        <v>59</v>
+      </c>
+      <c r="C69" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>60</v>
+      </c>
+      <c r="B70" t="s">
+        <v>60</v>
+      </c>
+      <c r="C70" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>61</v>
+      </c>
+      <c r="B71" t="s">
+        <v>61</v>
+      </c>
+      <c r="C71" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>62</v>
+      </c>
+      <c r="B72" t="s">
+        <v>62</v>
+      </c>
+      <c r="C72" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>63</v>
+      </c>
+      <c r="B73" t="s">
+        <v>63</v>
+      </c>
+      <c r="C73" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>150</v>
+      </c>
+      <c r="B74" t="s">
+        <v>150</v>
+      </c>
+      <c r="C74" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>151</v>
+      </c>
+      <c r="B75" t="s">
+        <v>151</v>
+      </c>
+      <c r="C75" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>68</v>
+      </c>
+      <c r="B76" t="s">
+        <v>68</v>
+      </c>
+      <c r="C76" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" t="s">
+        <v>152</v>
+      </c>
+      <c r="C77" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>153</v>
+      </c>
+      <c r="B78" t="s">
+        <v>153</v>
+      </c>
+      <c r="C78" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>154</v>
+      </c>
+      <c r="B79" t="s">
+        <v>154</v>
+      </c>
+      <c r="C79" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>155</v>
+      </c>
+      <c r="B80" t="s">
+        <v>155</v>
+      </c>
+      <c r="C80" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>156</v>
+      </c>
+      <c r="B81" t="s">
+        <v>156</v>
+      </c>
+      <c r="C81" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>157</v>
+      </c>
+      <c r="B82" t="s">
+        <v>157</v>
+      </c>
+      <c r="C82" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>158</v>
+      </c>
+      <c r="B83" t="s">
+        <v>158</v>
+      </c>
+      <c r="C83" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>159</v>
+      </c>
+      <c r="B84" t="s">
+        <v>159</v>
+      </c>
+      <c r="C84" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>160</v>
+      </c>
+      <c r="B85" t="s">
+        <v>160</v>
+      </c>
+      <c r="C85" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>161</v>
+      </c>
+      <c r="B86" t="s">
+        <v>161</v>
+      </c>
+      <c r="C86" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>162</v>
+      </c>
+      <c r="B87" t="s">
+        <v>162</v>
+      </c>
+      <c r="C87" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>163</v>
+      </c>
+      <c r="B88" t="s">
+        <v>163</v>
+      </c>
+      <c r="C88" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>164</v>
+      </c>
+      <c r="B89" t="s">
+        <v>164</v>
+      </c>
+      <c r="C89" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>165</v>
+      </c>
+      <c r="B90" t="s">
+        <v>165</v>
+      </c>
+      <c r="C90" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>166</v>
+      </c>
+      <c r="B91" t="s">
+        <v>166</v>
+      </c>
+      <c r="C91" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>167</v>
+      </c>
+      <c r="B92" t="s">
+        <v>167</v>
+      </c>
+      <c r="C92" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>168</v>
+      </c>
+      <c r="B93" t="s">
+        <v>168</v>
+      </c>
+      <c r="C93" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>169</v>
+      </c>
+      <c r="B94" t="s">
+        <v>169</v>
+      </c>
+      <c r="C94" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>170</v>
+      </c>
+      <c r="B95" t="s">
+        <v>170</v>
+      </c>
+      <c r="C95" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>171</v>
+      </c>
+      <c r="B96" t="s">
+        <v>171</v>
+      </c>
+      <c r="C96" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>172</v>
+      </c>
+      <c r="B97" t="s">
+        <v>172</v>
+      </c>
+      <c r="C97" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>173</v>
+      </c>
+      <c r="B98" t="s">
+        <v>173</v>
+      </c>
+      <c r="C98" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>174</v>
+      </c>
+      <c r="B99" t="s">
+        <v>174</v>
+      </c>
+      <c r="C99" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>175</v>
+      </c>
+      <c r="B100" t="s">
+        <v>175</v>
+      </c>
+      <c r="C100" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>176</v>
+      </c>
+      <c r="B101" t="s">
+        <v>176</v>
+      </c>
+      <c r="C101" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>177</v>
+      </c>
+      <c r="B102" t="s">
+        <v>177</v>
+      </c>
+      <c r="C102" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D102" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>178</v>
+      </c>
+      <c r="B103" t="s">
+        <v>178</v>
+      </c>
+      <c r="C103" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D103" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>179</v>
+      </c>
+      <c r="B104" t="s">
+        <v>179</v>
+      </c>
+      <c r="C104" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>180</v>
+      </c>
+      <c r="B105" t="s">
+        <v>180</v>
+      </c>
+      <c r="C105" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D105" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>97</v>
+      </c>
+      <c r="B106" t="s">
+        <v>97</v>
+      </c>
+      <c r="C106" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>181</v>
+      </c>
+      <c r="B107" t="s">
+        <v>181</v>
+      </c>
+      <c r="C107" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D107" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>182</v>
+      </c>
+      <c r="B108" t="s">
+        <v>182</v>
+      </c>
+      <c r="C108" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D108" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>183</v>
+      </c>
+      <c r="B109" t="s">
+        <v>183</v>
+      </c>
+      <c r="C109" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D109" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>184</v>
+      </c>
+      <c r="B110" t="s">
+        <v>184</v>
+      </c>
+      <c r="C110" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>102</v>
+      </c>
+      <c r="B111" t="s">
+        <v>102</v>
+      </c>
+      <c r="C111" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D108" xr:uid="{11956367-CD9C-EC4B-9F32-52680E70CD65}"/>
+  <conditionalFormatting sqref="C2:C121">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -9241,26 +11070,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE4332B-3F41-D74D-BC46-926B80854FC8}">
-  <dimension ref="A1:D108"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23CDF3A-ABF0-0E47-9203-6071B4EAE752}">
+  <dimension ref="A1:D111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="53.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.83203125" customWidth="1"/>
+    <col min="2" max="2" width="48.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>113</v>
+      <c r="A1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" t="s">
+        <v>189</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>106</v>
@@ -9270,7 +11099,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>122</v>
       </c>
       <c r="C2" t="b">
@@ -9278,12 +11107,12 @@
         <v>0</v>
       </c>
       <c r="D2" t="str">
-        <f>IF(A2=B2,"",IF(ISBLANK(A2),"DELETE","PUT"))</f>
-        <v>PUT</v>
+        <f>IF(A2=B2,"",IF(ISBLANK(B2),"PUT","DELETE"))</f>
+        <v>DELETE</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="b">
@@ -9291,12 +11120,12 @@
         <v>0</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D66" si="1">IF(A3=B3,"",IF(ISBLANK(A3),"DELETE","PUT"))</f>
-        <v>PUT</v>
+        <f t="shared" ref="D3:D66" si="1">IF(A3=B3,"",IF(ISBLANK(B3),"PUT","DELETE"))</f>
+        <v>DELETE</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>123</v>
       </c>
       <c r="C4" t="b">
@@ -9305,11 +11134,11 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
+        <v>DELETE</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>124</v>
       </c>
       <c r="C5" t="b">
@@ -9318,11 +11147,11 @@
       </c>
       <c r="D5" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
+        <v>DELETE</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>125</v>
       </c>
       <c r="C6" t="b">
@@ -9331,11 +11160,11 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
+        <v>DELETE</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>115</v>
       </c>
       <c r="C7" t="b">
@@ -9344,11 +11173,11 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
+        <v>DELETE</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>126</v>
       </c>
       <c r="C8" t="b">
@@ -9357,11 +11186,11 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
+        <v>DELETE</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="b">
@@ -9370,11 +11199,11 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
+        <v>DELETE</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="b">
@@ -9383,11 +11212,11 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
+        <v>DELETE</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="b">
@@ -9396,11 +11225,11 @@
       </c>
       <c r="D11" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
+        <v>DELETE</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="b">
@@ -9409,11 +11238,11 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
+        <v>DELETE</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13" t="b">
@@ -9422,11 +11251,11 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
+        <v>DELETE</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14" t="b">
@@ -9435,11 +11264,11 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
+        <v>DELETE</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="b">
@@ -9448,11 +11277,11 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
+        <v>DELETE</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="C16" t="b">
@@ -9461,11 +11290,11 @@
       </c>
       <c r="D16" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>16</v>
       </c>
       <c r="C17" t="b">
@@ -9474,11 +11303,11 @@
       </c>
       <c r="D17" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>17</v>
       </c>
       <c r="C18" t="b">
@@ -9487,11 +11316,11 @@
       </c>
       <c r="D18" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>116</v>
       </c>
       <c r="C19" t="b">
@@ -9500,11 +11329,11 @@
       </c>
       <c r="D19" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
         <v>117</v>
       </c>
       <c r="C20" t="b">
@@ -9513,11 +11342,11 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
         <v>118</v>
       </c>
       <c r="C21" t="b">
@@ -9526,11 +11355,11 @@
       </c>
       <c r="D21" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>19</v>
       </c>
       <c r="C22" t="b">
@@ -9539,11 +11368,11 @@
       </c>
       <c r="D22" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>127</v>
       </c>
       <c r="C23" t="b">
@@ -9552,11 +11381,11 @@
       </c>
       <c r="D23" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>128</v>
       </c>
       <c r="C24" t="b">
@@ -9565,11 +11394,11 @@
       </c>
       <c r="D24" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>129</v>
       </c>
       <c r="C25" t="b">
@@ -9578,11 +11407,11 @@
       </c>
       <c r="D25" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>23</v>
       </c>
       <c r="C26" t="b">
@@ -9591,11 +11420,11 @@
       </c>
       <c r="D26" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
         <v>24</v>
       </c>
       <c r="C27" t="b">
@@ -9604,1065 +11433,1103 @@
       </c>
       <c r="D27" t="str">
         <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>185</v>
+      </c>
+      <c r="C28" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>186</v>
+      </c>
+      <c r="C29" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>25</v>
       </c>
-      <c r="C28" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D28" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="C30" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>119</v>
       </c>
-      <c r="C29" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D29" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="C31" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
         <v>130</v>
       </c>
-      <c r="C30" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D30" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="C32" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
         <v>131</v>
       </c>
-      <c r="C31" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D31" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="C33" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
         <v>132</v>
       </c>
-      <c r="C32" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D32" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="C34" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
         <v>133</v>
       </c>
-      <c r="C33" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D33" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="C35" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
         <v>134</v>
       </c>
-      <c r="C34" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D34" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="C36" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
         <v>135</v>
       </c>
-      <c r="C35" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D35" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="C37" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
         <v>136</v>
       </c>
-      <c r="C36" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D36" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="C38" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
         <v>137</v>
       </c>
-      <c r="C37" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D37" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="C39" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
         <v>33</v>
       </c>
-      <c r="C38" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D38" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="C40" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
         <v>34</v>
       </c>
-      <c r="C39" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D39" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="C41" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
         <v>35</v>
       </c>
-      <c r="C40" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D40" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="C42" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
         <v>36</v>
       </c>
-      <c r="C41" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D41" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="C43" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
         <v>138</v>
       </c>
-      <c r="C42" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D42" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="C44" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
         <v>139</v>
       </c>
-      <c r="C43" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D43" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="C45" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
         <v>40</v>
       </c>
-      <c r="C44" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D44" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="C46" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
         <v>41</v>
       </c>
-      <c r="C45" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D45" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="C47" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
         <v>140</v>
       </c>
-      <c r="C46" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D46" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="C48" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
         <v>141</v>
       </c>
-      <c r="C47" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D47" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="C49" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
         <v>44</v>
       </c>
-      <c r="C48" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D48" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="C50" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
         <v>45</v>
       </c>
-      <c r="C49" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D49" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="C51" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
         <v>142</v>
       </c>
-      <c r="C50" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D50" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="C52" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
         <v>46</v>
       </c>
-      <c r="C51" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D51" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="C53" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>187</v>
+      </c>
+      <c r="C54" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
         <v>47</v>
       </c>
-      <c r="C52" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D52" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="C55" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
         <v>120</v>
       </c>
-      <c r="C53" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D53" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="C56" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
         <v>143</v>
       </c>
-      <c r="C54" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D54" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="C57" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
         <v>49</v>
       </c>
-      <c r="C55" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D55" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="C58" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
         <v>121</v>
       </c>
-      <c r="C56" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D56" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="C59" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
         <v>50</v>
       </c>
-      <c r="C57" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D57" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="C60" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
         <v>144</v>
       </c>
-      <c r="C58" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D58" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="C61" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
         <v>145</v>
       </c>
-      <c r="C59" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D59" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="C62" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
         <v>146</v>
       </c>
-      <c r="C60" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D60" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="C63" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
         <v>147</v>
       </c>
-      <c r="C61" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D61" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="C64" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
         <v>55</v>
       </c>
-      <c r="C62" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D62" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="C65" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
         <v>148</v>
       </c>
-      <c r="C63" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D63" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="C66" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="1"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
         <v>149</v>
       </c>
-      <c r="C64" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D64" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="C67" t="b">
+        <f t="shared" ref="C67:C111" si="2">A67=B67</f>
+        <v>0</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" ref="D67:D111" si="3">IF(A67=B67,"",IF(ISBLANK(B67),"PUT","DELETE"))</f>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
         <v>58</v>
       </c>
-      <c r="C65" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D65" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="C68" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
         <v>59</v>
       </c>
-      <c r="C66" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D66" t="str">
-        <f t="shared" si="1"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="C69" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
         <v>60</v>
       </c>
-      <c r="C67" t="b">
-        <f t="shared" ref="C67:C108" si="2">A67=B67</f>
-        <v>0</v>
-      </c>
-      <c r="D67" t="str">
-        <f t="shared" ref="D67:D108" si="3">IF(A67=B67,"",IF(ISBLANK(A67),"DELETE","PUT"))</f>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="C70" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
         <v>61</v>
       </c>
-      <c r="C68" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D68" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="C71" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
         <v>62</v>
       </c>
-      <c r="C69" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D69" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="C72" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
         <v>63</v>
       </c>
-      <c r="C70" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D70" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="C73" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
         <v>150</v>
       </c>
-      <c r="C71" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D71" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="C74" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
         <v>151</v>
       </c>
-      <c r="C72" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D72" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="C75" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
         <v>68</v>
       </c>
-      <c r="C73" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D73" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="C76" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
         <v>152</v>
       </c>
-      <c r="C74" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D74" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+      <c r="C77" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
         <v>153</v>
       </c>
-      <c r="C75" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D75" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="C78" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
         <v>154</v>
       </c>
-      <c r="C76" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D76" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+      <c r="C79" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B80" t="s">
         <v>155</v>
       </c>
-      <c r="C77" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D77" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+      <c r="C80" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
         <v>156</v>
       </c>
-      <c r="C78" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D78" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+      <c r="C81" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B82" t="s">
         <v>157</v>
       </c>
-      <c r="C79" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D79" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+      <c r="C82" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B83" t="s">
         <v>158</v>
       </c>
-      <c r="C80" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D80" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+      <c r="C83" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B84" t="s">
         <v>159</v>
       </c>
-      <c r="C81" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D81" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+      <c r="C84" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B85" t="s">
         <v>160</v>
       </c>
-      <c r="C82" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D82" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+      <c r="C85" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B86" t="s">
         <v>161</v>
       </c>
-      <c r="C83" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D83" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+      <c r="C86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
         <v>162</v>
       </c>
-      <c r="C84" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D84" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+      <c r="C87" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
         <v>163</v>
       </c>
-      <c r="C85" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D85" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+      <c r="C88" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
         <v>164</v>
       </c>
-      <c r="C86" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D86" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+      <c r="C89" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B90" t="s">
         <v>165</v>
       </c>
-      <c r="C87" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D87" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+      <c r="C90" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B91" t="s">
         <v>166</v>
       </c>
-      <c r="C88" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D88" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+      <c r="C91" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B92" t="s">
         <v>167</v>
       </c>
-      <c r="C89" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D89" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+      <c r="C92" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B93" t="s">
         <v>168</v>
       </c>
-      <c r="C90" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D90" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+      <c r="C93" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B94" t="s">
         <v>169</v>
       </c>
-      <c r="C91" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D91" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+      <c r="C94" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B95" t="s">
         <v>170</v>
       </c>
-      <c r="C92" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D92" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+      <c r="C95" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
         <v>171</v>
       </c>
-      <c r="C93" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D93" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+      <c r="C96" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
         <v>172</v>
       </c>
-      <c r="C94" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D94" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+      <c r="C97" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B98" t="s">
         <v>173</v>
       </c>
-      <c r="C95" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D95" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
+      <c r="C98" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B99" t="s">
         <v>174</v>
       </c>
-      <c r="C96" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D96" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
+      <c r="C99" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B100" t="s">
         <v>175</v>
       </c>
-      <c r="C97" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D97" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
+      <c r="C100" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B101" t="s">
         <v>176</v>
       </c>
-      <c r="C98" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D98" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
+      <c r="C101" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B102" t="s">
         <v>177</v>
       </c>
-      <c r="C99" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D99" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+      <c r="C102" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D102" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B103" t="s">
         <v>178</v>
       </c>
-      <c r="C100" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D100" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
+      <c r="C103" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D103" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B104" t="s">
         <v>179</v>
       </c>
-      <c r="C101" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D101" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
+      <c r="C104" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B105" t="s">
         <v>180</v>
       </c>
-      <c r="C102" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D102" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+      <c r="C105" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D105" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B106" t="s">
         <v>97</v>
       </c>
-      <c r="C103" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D103" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+      <c r="C106" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B107" t="s">
         <v>181</v>
       </c>
-      <c r="C104" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D104" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+      <c r="C107" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D107" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B108" t="s">
         <v>182</v>
       </c>
-      <c r="C105" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D105" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
+      <c r="C108" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D108" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B109" t="s">
         <v>183</v>
       </c>
-      <c r="C106" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D106" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+      <c r="C109" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D109" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B110" t="s">
         <v>184</v>
       </c>
-      <c r="C107" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D107" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+      <c r="C110" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B111" t="s">
         <v>102</v>
       </c>
-      <c r="C108" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D108" t="str">
-        <f t="shared" si="3"/>
-        <v>PUT</v>
+      <c r="C111" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="3"/>
+        <v>DELETE</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D108" xr:uid="{11956367-CD9C-EC4B-9F32-52680E70CD65}"/>
-  <conditionalFormatting sqref="C2:C108">
+  <conditionalFormatting sqref="C2:C121">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
Q search API completed
</commit_message>
<xml_diff>
--- a/doc/external-libraries.xlsx
+++ b/doc/external-libraries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandeep/projects/sconsole/SConsoleNxt/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8AF03F-2C31-AA43-B07C-36D172AA6245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA3E779-AF6A-1842-BA21-E54DA695E6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4780" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{A6983AAA-76E0-C546-86DD-E7128BD6E8D3}"/>
+    <workbookView xWindow="4780" yWindow="-21000" windowWidth="38400" windowHeight="21000" activeTab="6" xr2:uid="{A6983AAA-76E0-C546-86DD-E7128BD6E8D3}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 01 18" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1606" uniqueCount="191">
   <si>
     <t>Server Libs</t>
   </si>
@@ -639,6 +639,9 @@
   </si>
   <si>
     <t>Server</t>
+  </si>
+  <si>
+    <t>jakarta.validation-api-4.0.0-M1.jar</t>
   </si>
 </sst>
 </file>
@@ -9329,7 +9332,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="b">
-        <f t="shared" ref="C3:C66" si="0">A3=B3</f>
+        <f t="shared" ref="C3:C27" si="0">A3=B3</f>
         <v>1</v>
       </c>
       <c r="D3" t="str">
@@ -9726,7 +9729,7 @@
         <v>185</v>
       </c>
       <c r="C28" t="b">
-        <f t="shared" ref="C28:C91" si="2">A28=B28</f>
+        <f t="shared" ref="C28:C53" si="2">A28=B28</f>
         <v>0</v>
       </c>
       <c r="D28" t="str">
@@ -11072,10 +11075,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23CDF3A-ABF0-0E47-9203-6071B4EAE752}">
-  <dimension ref="A1:D111"/>
+  <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11099,1433 +11102,1776 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
       <c r="B2" t="s">
         <v>122</v>
       </c>
       <c r="C2" t="b">
         <f>A2=B2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="str">
         <f>IF(A2=B2,"",IF(ISBLANK(B2),"PUT","DELETE"))</f>
-        <v>DELETE</v>
+        <v/>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="b">
         <f t="shared" ref="C3:C66" si="0">A3=B3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D66" si="1">IF(A3=B3,"",IF(ISBLANK(B3),"PUT","DELETE"))</f>
-        <v>DELETE</v>
+        <v/>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
       <c r="B4" t="s">
         <v>123</v>
       </c>
       <c r="C4" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
       <c r="B5" t="s">
         <v>124</v>
       </c>
       <c r="C5" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
       <c r="B6" t="s">
         <v>125</v>
       </c>
       <c r="C6" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
       <c r="B7" t="s">
         <v>115</v>
       </c>
       <c r="C7" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>126</v>
+      </c>
       <c r="B8" t="s">
         <v>126</v>
       </c>
       <c r="C8" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="C16" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
       <c r="C17" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
       <c r="C18" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
       <c r="B19" t="s">
         <v>116</v>
       </c>
       <c r="C19" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>117</v>
+      </c>
       <c r="B20" t="s">
         <v>117</v>
       </c>
       <c r="C20" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>118</v>
+      </c>
       <c r="B21" t="s">
         <v>118</v>
       </c>
       <c r="C21" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
       <c r="B22" t="s">
         <v>19</v>
       </c>
       <c r="C22" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>127</v>
+      </c>
       <c r="B23" t="s">
         <v>127</v>
       </c>
       <c r="C23" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>128</v>
+      </c>
       <c r="B24" t="s">
         <v>128</v>
       </c>
       <c r="C24" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>129</v>
+      </c>
       <c r="B25" t="s">
         <v>129</v>
       </c>
       <c r="C25" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
       <c r="B26" t="s">
         <v>23</v>
       </c>
       <c r="C26" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
       <c r="B27" t="s">
         <v>24</v>
       </c>
       <c r="C27" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>185</v>
+      </c>
       <c r="B28" t="s">
         <v>185</v>
       </c>
       <c r="C28" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>186</v>
+      </c>
       <c r="B29" t="s">
         <v>186</v>
       </c>
       <c r="C29" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
       <c r="B30" t="s">
         <v>25</v>
       </c>
       <c r="C30" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>119</v>
+      </c>
       <c r="B31" t="s">
         <v>119</v>
       </c>
       <c r="C31" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>130</v>
+      </c>
       <c r="B32" t="s">
         <v>130</v>
       </c>
       <c r="C32" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>131</v>
+      </c>
       <c r="B33" t="s">
         <v>131</v>
       </c>
       <c r="C33" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>132</v>
+      </c>
       <c r="B34" t="s">
         <v>132</v>
       </c>
       <c r="C34" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>133</v>
+      </c>
       <c r="B35" t="s">
         <v>133</v>
       </c>
       <c r="C35" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>134</v>
+      </c>
       <c r="B36" t="s">
         <v>134</v>
       </c>
       <c r="C36" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>135</v>
+      </c>
       <c r="B37" t="s">
         <v>135</v>
       </c>
       <c r="C37" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>136</v>
+      </c>
       <c r="B38" t="s">
         <v>136</v>
       </c>
       <c r="C38" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>137</v>
+      </c>
       <c r="B39" t="s">
         <v>137</v>
       </c>
       <c r="C39" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>33</v>
+      </c>
       <c r="B40" t="s">
         <v>33</v>
       </c>
       <c r="C40" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>34</v>
+      </c>
       <c r="B41" t="s">
         <v>34</v>
       </c>
       <c r="C41" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>35</v>
+      </c>
       <c r="B42" t="s">
         <v>35</v>
       </c>
       <c r="C42" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>36</v>
+      </c>
       <c r="B43" t="s">
         <v>36</v>
       </c>
       <c r="C43" t="b">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>190</v>
+      </c>
+      <c r="C44" t="b">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D43" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
+      <c r="D44" t="str">
+        <f t="shared" si="1"/>
+        <v>PUT</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>138</v>
       </c>
-      <c r="C44" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D44" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>139</v>
       </c>
-      <c r="C45" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D45" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
+        <v>139</v>
+      </c>
+      <c r="C46" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>40</v>
       </c>
-      <c r="C46" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D46" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>41</v>
       </c>
-      <c r="C47" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D47" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>140</v>
       </c>
-      <c r="C48" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D48" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
+        <v>140</v>
+      </c>
+      <c r="C49" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>141</v>
       </c>
-      <c r="C49" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D49" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
+        <v>141</v>
+      </c>
+      <c r="C50" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>44</v>
       </c>
-      <c r="C50" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D50" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>45</v>
       </c>
-      <c r="C51" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D51" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>142</v>
       </c>
-      <c r="C52" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D52" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
+        <v>142</v>
+      </c>
+      <c r="C53" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>46</v>
       </c>
-      <c r="C53" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D53" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
+        <v>46</v>
+      </c>
+      <c r="C54" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>187</v>
       </c>
-      <c r="C54" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D54" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
+        <v>187</v>
+      </c>
+      <c r="C55" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>47</v>
       </c>
-      <c r="C55" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D55" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
+        <v>47</v>
+      </c>
+      <c r="C56" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>120</v>
       </c>
-      <c r="C56" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D56" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
+        <v>120</v>
+      </c>
+      <c r="C57" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>143</v>
       </c>
-      <c r="C57" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D57" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
+        <v>143</v>
+      </c>
+      <c r="C58" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>49</v>
       </c>
-      <c r="C58" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D58" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
+        <v>49</v>
+      </c>
+      <c r="C59" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>121</v>
       </c>
-      <c r="C59" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D59" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>50</v>
       </c>
-      <c r="C60" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D60" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
+        <v>50</v>
+      </c>
+      <c r="C61" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>144</v>
       </c>
-      <c r="C61" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D61" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
+        <v>144</v>
+      </c>
+      <c r="C62" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>145</v>
       </c>
-      <c r="C62" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D62" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
+        <v>145</v>
+      </c>
+      <c r="C63" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>146</v>
       </c>
-      <c r="C63" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D63" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
+        <v>146</v>
+      </c>
+      <c r="C64" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>147</v>
       </c>
-      <c r="C64" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D64" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
+        <v>147</v>
+      </c>
+      <c r="C65" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>55</v>
       </c>
-      <c r="C65" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D65" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
+        <v>55</v>
+      </c>
+      <c r="C66" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>148</v>
       </c>
-      <c r="C66" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D66" t="str">
-        <f t="shared" si="1"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
+        <v>148</v>
+      </c>
+      <c r="C67" t="b">
+        <f t="shared" ref="C67:C112" si="2">A67=B67</f>
+        <v>1</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" ref="D67:D112" si="3">IF(A67=B67,"",IF(ISBLANK(B67),"PUT","DELETE"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>149</v>
       </c>
-      <c r="C67" t="b">
-        <f t="shared" ref="C67:C111" si="2">A67=B67</f>
-        <v>0</v>
-      </c>
-      <c r="D67" t="str">
-        <f t="shared" ref="D67:D111" si="3">IF(A67=B67,"",IF(ISBLANK(B67),"PUT","DELETE"))</f>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
+        <v>149</v>
+      </c>
+      <c r="C68" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>58</v>
       </c>
-      <c r="C68" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D68" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
+        <v>58</v>
+      </c>
+      <c r="C69" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>59</v>
       </c>
-      <c r="C69" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D69" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
+        <v>59</v>
+      </c>
+      <c r="C70" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>60</v>
       </c>
-      <c r="C70" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D70" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
+        <v>60</v>
+      </c>
+      <c r="C71" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>61</v>
       </c>
-      <c r="C71" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D71" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
+        <v>61</v>
+      </c>
+      <c r="C72" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>62</v>
       </c>
-      <c r="C72" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D72" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
+        <v>62</v>
+      </c>
+      <c r="C73" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>63</v>
       </c>
-      <c r="C73" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D73" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
+        <v>63</v>
+      </c>
+      <c r="C74" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>150</v>
       </c>
-      <c r="C74" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D74" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
+        <v>150</v>
+      </c>
+      <c r="C75" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>151</v>
       </c>
-      <c r="C75" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D75" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
+        <v>151</v>
+      </c>
+      <c r="C76" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>68</v>
       </c>
-      <c r="C76" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D76" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
+        <v>68</v>
+      </c>
+      <c r="C77" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>152</v>
       </c>
-      <c r="C77" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D77" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
+        <v>152</v>
+      </c>
+      <c r="C78" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>153</v>
       </c>
-      <c r="C78" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D78" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
+        <v>153</v>
+      </c>
+      <c r="C79" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>154</v>
       </c>
-      <c r="C79" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D79" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
+        <v>154</v>
+      </c>
+      <c r="C80" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>155</v>
       </c>
-      <c r="C80" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D80" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
+        <v>155</v>
+      </c>
+      <c r="C81" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>156</v>
       </c>
-      <c r="C81" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D81" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
+        <v>156</v>
+      </c>
+      <c r="C82" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>157</v>
       </c>
-      <c r="C82" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D82" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
+        <v>157</v>
+      </c>
+      <c r="C83" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>158</v>
       </c>
-      <c r="C83" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D83" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
+        <v>158</v>
+      </c>
+      <c r="C84" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>159</v>
       </c>
-      <c r="C84" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D84" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
+        <v>159</v>
+      </c>
+      <c r="C85" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>160</v>
       </c>
-      <c r="C85" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D85" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
+        <v>160</v>
+      </c>
+      <c r="C86" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>161</v>
       </c>
-      <c r="C86" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D86" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
+        <v>161</v>
+      </c>
+      <c r="C87" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>162</v>
       </c>
-      <c r="C87" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D87" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
+        <v>162</v>
+      </c>
+      <c r="C88" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>163</v>
       </c>
-      <c r="C88" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D88" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
+        <v>163</v>
+      </c>
+      <c r="C89" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>164</v>
       </c>
-      <c r="C89" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D89" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
+        <v>164</v>
+      </c>
+      <c r="C90" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>165</v>
       </c>
-      <c r="C90" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D90" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
+        <v>165</v>
+      </c>
+      <c r="C91" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>166</v>
       </c>
-      <c r="C91" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D91" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
+        <v>166</v>
+      </c>
+      <c r="C92" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>167</v>
       </c>
-      <c r="C92" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D92" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
+        <v>167</v>
+      </c>
+      <c r="C93" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>168</v>
       </c>
-      <c r="C93" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D93" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
+        <v>168</v>
+      </c>
+      <c r="C94" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>169</v>
       </c>
-      <c r="C94" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D94" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
+        <v>169</v>
+      </c>
+      <c r="C95" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>170</v>
       </c>
-      <c r="C95" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D95" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
+        <v>170</v>
+      </c>
+      <c r="C96" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>171</v>
       </c>
-      <c r="C96" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D96" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
+        <v>171</v>
+      </c>
+      <c r="C97" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
         <v>172</v>
       </c>
-      <c r="C97" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D97" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
+        <v>172</v>
+      </c>
+      <c r="C98" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
         <v>173</v>
       </c>
-      <c r="C98" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D98" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
+        <v>173</v>
+      </c>
+      <c r="C99" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>174</v>
       </c>
-      <c r="C99" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D99" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
+        <v>174</v>
+      </c>
+      <c r="C100" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>175</v>
       </c>
-      <c r="C100" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D100" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
+        <v>175</v>
+      </c>
+      <c r="C101" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
         <v>176</v>
       </c>
-      <c r="C101" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D101" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
+        <v>176</v>
+      </c>
+      <c r="C102" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D102" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>177</v>
       </c>
-      <c r="C102" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D102" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
+        <v>177</v>
+      </c>
+      <c r="C103" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D103" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>178</v>
       </c>
-      <c r="C103" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D103" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
+        <v>178</v>
+      </c>
+      <c r="C104" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
         <v>179</v>
       </c>
-      <c r="C104" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D104" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
+        <v>179</v>
+      </c>
+      <c r="C105" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D105" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>180</v>
       </c>
-      <c r="C105" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D105" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
+        <v>180</v>
+      </c>
+      <c r="C106" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>97</v>
       </c>
-      <c r="C106" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D106" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
+        <v>97</v>
+      </c>
+      <c r="C107" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D107" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>181</v>
       </c>
-      <c r="C107" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D107" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
+        <v>181</v>
+      </c>
+      <c r="C108" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D108" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>182</v>
       </c>
-      <c r="C108" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D108" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
+        <v>182</v>
+      </c>
+      <c r="C109" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D109" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>183</v>
       </c>
-      <c r="C109" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D109" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
+        <v>183</v>
+      </c>
+      <c r="C110" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>184</v>
       </c>
-      <c r="C110" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D110" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
-      </c>
-    </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
+        <v>184</v>
+      </c>
+      <c r="C111" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>102</v>
       </c>
-      <c r="C111" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D111" t="str">
-        <f t="shared" si="3"/>
-        <v>DELETE</v>
+      <c r="B112" t="s">
+        <v>102</v>
+      </c>
+      <c r="C112" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D112" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -12538,5 +12884,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>